<commit_message>
Changed the way to differentiate square and diamond, accuracy up to 85%
</commit_message>
<xml_diff>
--- a/Assignment2_Vision_Decorations/Test Results.xlsx
+++ b/Assignment2_Vision_Decorations/Test Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kevinly Santoso\Documents\UNI\y4s2\MTRN4230\Assignments\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984B6176-C60D-45A6-A747-5EF507945FD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A109D-21C5-4544-AE31-64C34471615F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="696" windowWidth="13620" windowHeight="6648" xr2:uid="{D096D856-D00E-42A3-869B-2EFCE23C768C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D096D856-D00E-42A3-869B-2EFCE23C768C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Test Results</t>
   </si>
@@ -54,19 +54,25 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>square interpreted as diamond and vice versa</t>
-  </si>
-  <si>
-    <t>green glare makes it really bad (only 50% of green correct)</t>
-  </si>
-  <si>
-    <t>green glare makes it really bad (only 50% of green correct), square interpreted as diamond</t>
-  </si>
-  <si>
-    <t>square interpreted as diamond, green glare</t>
-  </si>
-  <si>
-    <t>square interpreted as diamond</t>
+    <t>green and red glare makes it really bad</t>
+  </si>
+  <si>
+    <t>green glare</t>
+  </si>
+  <si>
+    <t>green glare, mask is really bad</t>
+  </si>
+  <si>
+    <t>green glare, blue 6 star interpreted as 4 star</t>
+  </si>
+  <si>
+    <t>red 4star interpreted as 6 star, green glare a square green was missed</t>
+  </si>
+  <si>
+    <t>red 4star interpreted as 6 star, green glare a square green was missed, green 4 star itnerpreted as 6star due to glare</t>
+  </si>
+  <si>
+    <t>green glare makes flower look like 6 star, square green missed cause of glare, blue square interpreted as flower due to perimeter</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5353C164-4D3E-4590-8810-058B4E8B57FF}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +487,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -489,13 +495,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D22" si="0">B5/C5</f>
+        <f t="shared" ref="D5:D27" si="0">B5/C5</f>
         <v>1</v>
       </c>
     </row>
@@ -519,17 +525,17 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>13</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0.76923076923076927</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -537,17 +543,17 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>15</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -555,17 +561,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>15</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.8</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -583,7 +589,7 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -591,17 +597,17 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>15</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -609,14 +615,14 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>0.8125</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -627,26 +633,161 @@
         <v>10</v>
       </c>
       <c r="B13" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.8125</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1">
+        <f>B25/C25</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" ref="D26:D27" si="1">B26/C26</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
-        <f>AVERAGE(D4:D13)</f>
-        <v>0.80608974358974361</v>
+      <c r="D31" s="1">
+        <f>AVERAGE(D4:D30)</f>
+        <v>0.85012233953410443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>